<commit_message>
Added new features to gantt chart
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Dropbox\School\Spring 22 - CMPE 131 Software Engineering\CMPE131-Spring22-Team4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anh Thu Pham\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F15996A-9A9B-41EC-A881-19538A871E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B535CB1-440E-491A-A07C-FFC21AC4ADFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Project Planner</t>
   </si>
@@ -228,7 +228,13 @@
     <t>Maintain UI Consistency</t>
   </si>
   <si>
-    <t>Add pictures for Items</t>
+    <t>Add Item Categories</t>
+  </si>
+  <si>
+    <t>View Purchase History</t>
+  </si>
+  <si>
+    <t>Add Pictures to Items</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -596,6 +602,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="11" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -643,12 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="11" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -672,7 +678,233 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1059,24 +1291,24 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="B1:BO32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="72" zoomScaleNormal="72" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="23.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.58203125" customWidth="1"/>
+    <col min="2" max="2" width="23.58203125" style="2" customWidth="1"/>
     <col min="3" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="4" customWidth="1"/>
     <col min="8" max="10" width="4.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="3.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="27" width="4.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1086,14 +1318,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1101,122 +1333,134 @@
         <v>56</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="31"/>
+      <c r="V2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="32" t="s">
+      <c r="AA2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="34"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="18"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AI2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-    </row>
-    <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+    </row>
+    <row r="3" spans="2:67" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="19">
         <v>44679</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="19">
         <v>44680</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="19">
         <v>44681</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="19">
         <v>44682</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3" s="19">
         <v>44683</v>
       </c>
-      <c r="M3" s="35">
+      <c r="M3" s="19">
         <v>44684</v>
       </c>
-      <c r="N3" s="35">
+      <c r="N3" s="19">
         <v>44685</v>
       </c>
-      <c r="O3" s="35">
+      <c r="O3" s="19">
         <v>44686</v>
       </c>
-      <c r="P3" s="35">
+      <c r="P3" s="19">
         <v>44687</v>
       </c>
-      <c r="Q3" s="35">
+      <c r="Q3" s="19">
         <v>44688</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="19">
         <v>44689</v>
       </c>
-      <c r="S3" s="35">
+      <c r="S3" s="19">
         <v>44690</v>
       </c>
-      <c r="T3" s="35">
+      <c r="T3" s="19">
         <v>44691</v>
       </c>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-    </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="U3" s="19">
+        <v>44692</v>
+      </c>
+      <c r="V3" s="19">
+        <v>44693</v>
+      </c>
+      <c r="W3" s="19">
+        <v>44694</v>
+      </c>
+      <c r="X3" s="19">
+        <v>44695</v>
+      </c>
+      <c r="Y3" s="19">
+        <v>44696</v>
+      </c>
+      <c r="Z3" s="19">
+        <v>44697</v>
+      </c>
+      <c r="AA3" s="19"/>
+    </row>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1398,8 +1642,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="s">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="7">
@@ -1418,8 +1662,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36" t="s">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="7">
@@ -1438,8 +1682,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="7">
@@ -1458,8 +1702,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="7">
@@ -1478,8 +1722,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="7">
@@ -1495,11 +1739,11 @@
         <v>4</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="7">
@@ -1515,11 +1759,11 @@
         <v>4</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="7">
@@ -1535,11 +1779,11 @@
         <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="7">
@@ -1549,17 +1793,17 @@
         <v>4</v>
       </c>
       <c r="E12" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="36" t="s">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="7">
@@ -1575,11 +1819,11 @@
         <v>4</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="20" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="7">
@@ -1598,8 +1842,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="9">
@@ -1618,18 +1862,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36" t="s">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D16" s="7">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
@@ -1638,18 +1882,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="20" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17" s="7">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F17" s="7">
         <v>4</v>
@@ -1658,18 +1902,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36" t="s">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18" s="7">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E18" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F18" s="7">
         <v>4</v>
@@ -1678,8 +1922,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="36" t="s">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="20" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="7">
@@ -1698,15 +1942,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36" t="s">
-        <v>39</v>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="7">
         <v>7</v>
       </c>
       <c r="D20" s="7">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E20" s="7">
         <v>7</v>
@@ -1718,58 +1962,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>14</v>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D21" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E21" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F21" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="C22" s="7">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D22" s="7">
-        <v>6</v>
-      </c>
-      <c r="E22" s="7">
-        <v>12</v>
-      </c>
-      <c r="F22" s="7">
-        <v>7</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="7">
         <v>5</v>
@@ -1778,143 +2018,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F24" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D25" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E25" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F25" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G25" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="7">
         <v>14</v>
       </c>
       <c r="D26" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E26" s="7">
         <v>14</v>
       </c>
       <c r="F26" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G26" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G27" s="8">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="7">
         <v>3</v>
       </c>
       <c r="G28" s="8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="7">
         <v>15</v>
       </c>
       <c r="D29" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E29" s="7">
         <v>15</v>
       </c>
       <c r="F29" s="7">
+        <v>8</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="7">
+        <v>15</v>
+      </c>
+      <c r="D30" s="7">
         <v>5</v>
       </c>
-      <c r="G29" s="8">
+      <c r="E30" s="7">
+        <v>15</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="7">
+        <v>15</v>
+      </c>
+      <c r="D31" s="7">
+        <v>8</v>
+      </c>
+      <c r="E31" s="7">
+        <v>15</v>
+      </c>
+      <c r="F31" s="7">
+        <v>5</v>
+      </c>
+      <c r="G31" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
+    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C32" s="7">
         <v>16</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D32" s="7">
         <v>28</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E32" s="7">
         <v>16</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F32" s="7">
         <v>30</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G32" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -1934,40 +2214,92 @@
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="H5:BO30">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="H5:BO19 H22:BO32">
+    <cfRule type="expression" dxfId="25" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="22" priority="21">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="18" priority="28">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BO31">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B33:BO33">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:BO20">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:BO21">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">

</xml_diff>

<commit_message>
Updated Gantt Chart dates and who's implementing
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anh Thu Pham\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anh Thu Pham\Desktop\Spring 2022\CMPE 131\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B535CB1-440E-491A-A07C-FFC21AC4ADFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500C4A45-8916-4B47-A937-3B7D26A471ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,58 +183,58 @@
     <t>Feature 26</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Create New Account</t>
-  </si>
-  <si>
-    <t>Delete Account</t>
-  </si>
-  <si>
-    <t>Update Account</t>
-  </si>
-  <si>
-    <t>Forgot Password</t>
-  </si>
-  <si>
-    <t>Seller Create Item</t>
-  </si>
-  <si>
-    <t>Seller Update Item</t>
-  </si>
-  <si>
-    <t>Seller Delete Item</t>
-  </si>
-  <si>
-    <t>View All Items</t>
-  </si>
-  <si>
-    <t>View Single Item</t>
-  </si>
-  <si>
-    <t>Add Item to Cart</t>
-  </si>
-  <si>
-    <t>Remove Items from Cart</t>
-  </si>
-  <si>
-    <t>Buy Items from Cart</t>
-  </si>
-  <si>
-    <t>Maintain UI Consistency</t>
-  </si>
-  <si>
-    <t>Add Item Categories</t>
-  </si>
-  <si>
-    <t>View Purchase History</t>
-  </si>
-  <si>
-    <t>Add Pictures to Items</t>
+    <t>Login - Nhan</t>
+  </si>
+  <si>
+    <t>Logout - Nhan</t>
+  </si>
+  <si>
+    <t>Create New Account - Nhan</t>
+  </si>
+  <si>
+    <t>Delete Account - Nhan</t>
+  </si>
+  <si>
+    <t>Update Account - Nhan</t>
+  </si>
+  <si>
+    <t>Forgot Password - Nhan</t>
+  </si>
+  <si>
+    <t>Seller Create Item - Aaron</t>
+  </si>
+  <si>
+    <t>Seller Update Item - Aaron</t>
+  </si>
+  <si>
+    <t>Seller Delete Item - Aaron</t>
+  </si>
+  <si>
+    <t>View All Items - Aaron</t>
+  </si>
+  <si>
+    <t>View Single Item - Aaron</t>
+  </si>
+  <si>
+    <t>Add Item Categories - Aaron</t>
+  </si>
+  <si>
+    <t>Add Item to Cart - Anh</t>
+  </si>
+  <si>
+    <t>Remove Items from Cart - Anh</t>
+  </si>
+  <si>
+    <t>Buy Items from Cart - Anh</t>
+  </si>
+  <si>
+    <t>Maintain UI Consistency - Nhan</t>
+  </si>
+  <si>
+    <t>Add Pictures to Items - Anh</t>
+  </si>
+  <si>
+    <t>View Purchase History - Aaron</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,233 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1294,13 +1520,13 @@
   <dimension ref="B1:BO32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="72" zoomScaleNormal="72" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="23.58203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.9140625" style="2" customWidth="1"/>
     <col min="3" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="4" customWidth="1"/>
     <col min="8" max="10" width="4.25" style="1" bestFit="1" customWidth="1"/>
@@ -1864,7 +2090,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="7">
         <v>4</v>
@@ -1876,55 +2102,47 @@
         <v>6</v>
       </c>
       <c r="F16" s="7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D17" s="7">
         <v>13</v>
       </c>
-      <c r="E17" s="7">
-        <v>6</v>
-      </c>
-      <c r="F17" s="7">
-        <v>4</v>
-      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D18" s="7">
-        <v>14</v>
-      </c>
-      <c r="E18" s="7">
-        <v>6</v>
-      </c>
-      <c r="F18" s="7">
-        <v>4</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
@@ -1939,18 +2157,18 @@
         <v>13</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C20" s="7">
         <v>7</v>
       </c>
       <c r="D20" s="7">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E20" s="7">
         <v>7</v>
@@ -1959,38 +2177,34 @@
         <v>7</v>
       </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D21" s="7">
-        <v>7</v>
-      </c>
-      <c r="E21" s="7">
-        <v>7</v>
-      </c>
-      <c r="F21" s="7">
-        <v>7</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D22" s="7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2214,69 +2428,69 @@
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="H5:BO19 H22:BO32">
-    <cfRule type="expression" dxfId="25" priority="17">
+  <conditionalFormatting sqref="H22:BO32 H5:BO19">
+    <cfRule type="expression" dxfId="41" priority="33">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="19">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="20">
+    <cfRule type="expression" dxfId="39" priority="36">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="38" priority="37">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="36" priority="39">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="27">
+    <cfRule type="expression" dxfId="35" priority="43">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="28">
+    <cfRule type="expression" dxfId="34" priority="44">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:BO33">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:BO20">
-    <cfRule type="expression" dxfId="15" priority="9">
+  <conditionalFormatting sqref="H21:BO21">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="30" priority="26">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="29" priority="27">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="28" priority="28">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="25" priority="31">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:BO21">
+  <conditionalFormatting sqref="H20:BO20">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>